<commit_message>
added visuals to high-level page
</commit_message>
<xml_diff>
--- a/Connected Office Dataset.xlsx
+++ b/Connected Office Dataset.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25825"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B83DBD73-BEF9-4406-B81F-1429B7E5DF6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dennis.VanTonder\Documents\GitHub\CMPG-323-Project-5-31609988\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2D216C-1D40-448E-9A25-E3A4D1303050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zone" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,7 @@
     <sheet name="Category" sheetId="3" r:id="rId3"/>
     <sheet name="Sub-Category" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -322,7 +327,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -798,14 +803,14 @@
       <selection sqref="A1:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -816,7 +821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -827,7 +832,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -838,7 +843,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -849,7 +854,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -860,7 +865,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
@@ -871,7 +876,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -882,7 +887,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
@@ -893,7 +898,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -904,7 +909,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
@@ -924,22 +929,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08439157-EFCA-47CB-8108-F53748A39E5E}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -962,7 +967,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
@@ -985,7 +990,7 @@
         <v>43855</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>40</v>
       </c>
@@ -1008,7 +1013,7 @@
         <v>44229</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>44</v>
       </c>
@@ -1031,7 +1036,7 @@
         <v>44541</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>47</v>
       </c>
@@ -1054,7 +1059,7 @@
         <v>44641</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>50</v>
       </c>
@@ -1077,7 +1082,7 @@
         <v>44641</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>52</v>
       </c>
@@ -1100,7 +1105,7 @@
         <v>44333</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>55</v>
       </c>
@@ -1123,7 +1128,7 @@
         <v>44409</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>56</v>
       </c>
@@ -1146,7 +1151,7 @@
         <v>44434</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>58</v>
       </c>
@@ -1180,14 +1185,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1198,7 +1203,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>62</v>
       </c>
@@ -1209,7 +1214,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>65</v>
       </c>
@@ -1220,7 +1225,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>68</v>
       </c>
@@ -1231,7 +1236,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>71</v>
       </c>
@@ -1242,7 +1247,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>74</v>
       </c>
@@ -1253,7 +1258,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>77</v>
       </c>
@@ -1264,7 +1269,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>80</v>
       </c>
@@ -1284,19 +1289,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC903D32-5F9E-4786-89D6-996B7E75E220}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1310,7 +1315,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>85</v>
       </c>
@@ -1324,7 +1329,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>87</v>
       </c>
@@ -1338,7 +1343,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>89</v>
       </c>
@@ -1352,7 +1357,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>91</v>
       </c>
@@ -1366,7 +1371,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>93</v>
       </c>
@@ -1386,26 +1391,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7a090801-4708-43a5-9598-e4e2166c002c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="4f4a8c57-659f-4264-b765-bd165a88863b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A38BD02CE626854CB2A69241B23A3E9B" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3995f0f3d16fb037e2c25f34d1e51555">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7a090801-4708-43a5-9598-e4e2166c002c" xmlns:ns3="4f4a8c57-659f-4264-b765-bd165a88863b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="66ec43485dfc5a4a75bbf1242e9d13e6" ns2:_="" ns3:_="">
     <xsd:import namespace="7a090801-4708-43a5-9598-e4e2166c002c"/>
@@ -1628,14 +1613,60 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7a090801-4708-43a5-9598-e4e2166c002c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="4f4a8c57-659f-4264-b765-bd165a88863b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B45281D-5D5A-4087-8014-4B4FA16E83A5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B6EE518-5DC1-4AFD-B150-7E05CC0C76D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7a090801-4708-43a5-9598-e4e2166c002c"/>
+    <ds:schemaRef ds:uri="4f4a8c57-659f-4264-b765-bd165a88863b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A227DC9-4D6F-4F55-89DE-623758C7FB72}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A227DC9-4D6F-4F55-89DE-623758C7FB72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B6EE518-5DC1-4AFD-B150-7E05CC0C76D1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B45281D-5D5A-4087-8014-4B4FA16E83A5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7a090801-4708-43a5-9598-e4e2166c002c"/>
+    <ds:schemaRef ds:uri="4f4a8c57-659f-4264-b765-bd165a88863b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added more test data to excel file
</commit_message>
<xml_diff>
--- a/Connected Office Dataset.xlsx
+++ b/Connected Office Dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dennis.VanTonder\Documents\GitHub\CMPG-323-Project-5-31609988\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2D216C-1D40-448E-9A25-E3A4D1303050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C7710B-07BE-45B0-908C-630460D691C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zone" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="107">
   <si>
     <t>ID</t>
   </si>
@@ -321,6 +321,42 @@
   </si>
   <si>
     <t>Measuring speed of moving object</t>
+  </si>
+  <si>
+    <t>SC06</t>
+  </si>
+  <si>
+    <t>Router to communitcate to internet</t>
+  </si>
+  <si>
+    <t>SC07</t>
+  </si>
+  <si>
+    <t>Communication device</t>
+  </si>
+  <si>
+    <t>Finger print sensor</t>
+  </si>
+  <si>
+    <t>Reader to authenticate users</t>
+  </si>
+  <si>
+    <t>SC08</t>
+  </si>
+  <si>
+    <t>Face scanner</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>Fingerprint reader</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>Face reader</t>
   </si>
 </sst>
 </file>
@@ -352,6 +388,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -370,7 +407,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -465,11 +502,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -483,6 +540,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,7 +861,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -927,10 +988,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08439157-EFCA-47CB-8108-F53748A39E5E}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1172,6 +1233,52 @@
       </c>
       <c r="G10" s="12">
         <v>44584</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" s="16">
+        <v>43917</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" s="16">
+        <v>43727</v>
       </c>
     </row>
   </sheetData>
@@ -1287,10 +1394,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC903D32-5F9E-4786-89D6-996B7E75E220}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1385,12 +1492,74 @@
         <v>94</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7a090801-4708-43a5-9598-e4e2166c002c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="4f4a8c57-659f-4264-b765-bd165a88863b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A38BD02CE626854CB2A69241B23A3E9B" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3995f0f3d16fb037e2c25f34d1e51555">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7a090801-4708-43a5-9598-e4e2166c002c" xmlns:ns3="4f4a8c57-659f-4264-b765-bd165a88863b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="66ec43485dfc5a4a75bbf1242e9d13e6" ns2:_="" ns3:_="">
     <xsd:import namespace="7a090801-4708-43a5-9598-e4e2166c002c"/>
@@ -1613,27 +1782,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B45281D-5D5A-4087-8014-4B4FA16E83A5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7a090801-4708-43a5-9598-e4e2166c002c"/>
+    <ds:schemaRef ds:uri="4f4a8c57-659f-4264-b765-bd165a88863b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7a090801-4708-43a5-9598-e4e2166c002c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="4f4a8c57-659f-4264-b765-bd165a88863b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A227DC9-4D6F-4F55-89DE-623758C7FB72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B6EE518-5DC1-4AFD-B150-7E05CC0C76D1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1650,23 +1818,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A227DC9-4D6F-4F55-89DE-623758C7FB72}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B45281D-5D5A-4087-8014-4B4FA16E83A5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7a090801-4708-43a5-9598-e4e2166c002c"/>
-    <ds:schemaRef ds:uri="4f4a8c57-659f-4264-b765-bd165a88863b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>